<commit_message>
Refining Variable Importance Analysis
Added logic for calculating the average change in odds ratio (of experiencing SICR-event relative to not experiencing it). Meant to enrich discussion in Appendix A.3 in article.
</commit_message>
<xml_diff>
--- a/General/Def1a(i)-(iv) - Goodman ranks.xlsx
+++ b/General/Def1a(i)-(iv) - Goodman ranks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://firstrandgroup-my.sharepoint.com/personal/f5361079_fnb_co_za/Documents/Github/IFRS9-SICR-Definitions-Logit/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkLife\Analytix\Research\Dynamic-SICR\IFRS9-SICR-Definitions-Logit\General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8595A0D0-0D74-413D-90E4-85CFC847D4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2845D6C0-135D-4EBC-9D51-9DED9B8D1D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A7BB07D9-9673-4827-8104-1170E3FF36F5}"/>
+    <workbookView xWindow="26130" yWindow="2865" windowWidth="34830" windowHeight="18885" xr2:uid="{A7BB07D9-9673-4827-8104-1170E3FF36F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>SICR_definition</t>
   </si>
@@ -108,13 +108,19 @@
   </si>
   <si>
     <t>Inflation_Growth</t>
+  </si>
+  <si>
+    <t>Effects deliberately discussed in analysis</t>
+  </si>
+  <si>
+    <t>Legend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,13 +128,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,8 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,9 +186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,7 +226,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -309,7 +332,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -459,36 +482,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6AFB46-1D9E-4C17-90E7-4E48A51AB171}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -609,7 +632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -668,7 +691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -724,7 +747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -779,6 +802,93 @@
       <c r="S5">
         <v>17</v>
       </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f>AVERAGE(B2:B5)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ref="C6:S6" si="0">AVERAGE(C2:C5)</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.25</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
+        <v>12.75</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.25</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.75</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>